<commit_message>
All primary electronics mounted.
Moved purchased hardware to dedicated directory.

FInally got rid of references to outer_drive_right by adding the missing parameter to parameters.xlsx.
</commit_message>
<xml_diff>
--- a/Mechanical CAD/parameters.xlsx
+++ b/Mechanical CAD/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rackstation\media\documents\Inventor\AutoBuoy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\CreekFleet_AutoBuoy\Mechanical CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16937E7A-053C-44F9-8E6F-3595B1C04D70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED12D58-698D-4D70-9609-20F956B6A5E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>parameter name</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>motor_shaft_key</t>
+  </si>
+  <si>
+    <t>slab_thick</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -761,6 +764,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>1.365</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>